<commit_message>
Add test excel, Data
</commit_message>
<xml_diff>
--- a/Data/data_users.xlsx
+++ b/Data/data_users.xlsx
@@ -26,10 +26,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
-    <t>mcarmen</t>
-  </si>
-  <si>
-    <t>Kiu3irSistemasTech.</t>
+    <t>yhernandez</t>
+  </si>
+  <si>
+    <t>Performance23!</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>busqueda_a</t>
@@ -39,25 +45,23 @@
   </si>
   <si>
     <t>hotmail</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,47 +372,42 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:XFD1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test case incompleto a verificar
</commit_message>
<xml_diff>
--- a/Data/data_users.xlsx
+++ b/Data/data_users.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smavodev\Desktop\playwright_python\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos_Demo\playwright_python_evolta\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCECFF3-660D-41CA-9DBA-72AD123BB53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13830" windowHeight="5625"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,16 +42,16 @@
     <t>busqueda_a</t>
   </si>
   <si>
+    <t>hotmail</t>
+  </si>
+  <si>
     <t>gmail</t>
-  </si>
-  <si>
-    <t>hotmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -368,14 +369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -412,6 +413,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>